<commit_message>
Change files for testing!
</commit_message>
<xml_diff>
--- a/source/column_and_variable_names/column_names.xlsx
+++ b/source/column_and_variable_names/column_names.xlsx
@@ -351,7 +351,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:B227"/>
+  <dimension ref="A1:B277"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -386,125 +386,215 @@
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>_NAME_</t>
+          <t>_015000</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>Up to £15,000</t>
         </is>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>£10,001 to £15,000</t>
+          <t>_06000</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>Up to £6,000</t>
         </is>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>£10,001 to £20,000</t>
+          <t>_1000115000</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>£10,001 to £15,000</t>
         </is>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>£20,001 to £25,000</t>
+          <t>_1000120000</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>£10,001 to £20,000</t>
         </is>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>£20,001 to £30,000</t>
+          <t>_120mostdeprived</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>1 - 20% most deprived</t>
         </is>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>£25,001 to £30,000</t>
+          <t>_120mostdeprived</t>
+        </is>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>1 - 20% most deprived</t>
         </is>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>£30,001 to £40,001</t>
+          <t>_120MostDeprived</t>
+        </is>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>1 - 20% most deprived</t>
         </is>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>£6,001 to £10,000</t>
+          <t>_14</t>
+        </is>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>14</t>
         </is>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>1 - 20% most deprived</t>
+          <t>_1500120000</t>
+        </is>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>1500120000</t>
         </is>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>14</t>
+          <t>_1500130000</t>
+        </is>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>1500130000</t>
         </is>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>1500120000</t>
+          <t>_1624</t>
+        </is>
+      </c>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>16 to 24</t>
         </is>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>1500130000</t>
+          <t>_1639</t>
+        </is>
+      </c>
+      <c r="B15" t="inlineStr">
+        <is>
+          <t>16 to 39</t>
         </is>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>16 to 24</t>
+          <t>_16to34</t>
+        </is>
+      </c>
+      <c r="B16" t="inlineStr">
+        <is>
+          <t>16 to 34</t>
         </is>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>16 to 34</t>
+          <t>_16to39</t>
+        </is>
+      </c>
+      <c r="B17" t="inlineStr">
+        <is>
+          <t>16 to 39</t>
         </is>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>16 to 39</t>
+          <t>_1999</t>
+        </is>
+      </c>
+      <c r="B18" t="inlineStr">
+        <is>
+          <t>1999</t>
         </is>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>1999</t>
+          <t>_19992000</t>
+        </is>
+      </c>
+      <c r="B19" t="inlineStr">
+        <is>
+          <t>1999/2000</t>
         </is>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>1999/2000</t>
+          <t>_1MostDeprived</t>
+        </is>
+      </c>
+      <c r="B20" t="inlineStr">
+        <is>
+          <t>1 - 20% most deprived</t>
         </is>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
+          <t>_2</t>
+        </is>
+      </c>
+      <c r="B21" t="inlineStr">
+        <is>
           <t>2</t>
         </is>
       </c>
@@ -512,27 +602,47 @@
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>20% least deprived</t>
+          <t>_2000</t>
+        </is>
+      </c>
+      <c r="B22" t="inlineStr">
+        <is>
+          <t>2000</t>
         </is>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>20% most deprived</t>
+          <t>_2000125000</t>
+        </is>
+      </c>
+      <c r="B23" t="inlineStr">
+        <is>
+          <t>£20,001 to £25,000</t>
         </is>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>2000</t>
+          <t>_2000130000</t>
+        </is>
+      </c>
+      <c r="B24" t="inlineStr">
+        <is>
+          <t>£20,001 to £30,000</t>
         </is>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
+          <t>_2001</t>
+        </is>
+      </c>
+      <c r="B25" t="inlineStr">
+        <is>
           <t>2001</t>
         </is>
       </c>
@@ -540,6 +650,11 @@
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
+          <t>_20012002</t>
+        </is>
+      </c>
+      <c r="B26" t="inlineStr">
+        <is>
           <t>2001/2002</t>
         </is>
       </c>
@@ -547,6 +662,11 @@
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
+          <t>_2002</t>
+        </is>
+      </c>
+      <c r="B27" t="inlineStr">
+        <is>
           <t>2002</t>
         </is>
       </c>
@@ -554,6 +674,11 @@
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
+          <t>_2003</t>
+        </is>
+      </c>
+      <c r="B28" t="inlineStr">
+        <is>
           <t>2003</t>
         </is>
       </c>
@@ -561,6 +686,11 @@
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
+          <t>_20032004</t>
+        </is>
+      </c>
+      <c r="B29" t="inlineStr">
+        <is>
           <t>2003/2004</t>
         </is>
       </c>
@@ -568,6 +698,11 @@
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
+          <t>_2004</t>
+        </is>
+      </c>
+      <c r="B30" t="inlineStr">
+        <is>
           <t>2004</t>
         </is>
       </c>
@@ -575,6 +710,11 @@
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
+          <t>_2005</t>
+        </is>
+      </c>
+      <c r="B31" t="inlineStr">
+        <is>
           <t>2005</t>
         </is>
       </c>
@@ -582,6 +722,11 @@
     <row r="32">
       <c r="A32" t="inlineStr">
         <is>
+          <t>_20052006</t>
+        </is>
+      </c>
+      <c r="B32" t="inlineStr">
+        <is>
           <t>2005/2006</t>
         </is>
       </c>
@@ -589,6 +734,11 @@
     <row r="33">
       <c r="A33" t="inlineStr">
         <is>
+          <t>_2006</t>
+        </is>
+      </c>
+      <c r="B33" t="inlineStr">
+        <is>
           <t>2006</t>
         </is>
       </c>
@@ -596,6 +746,11 @@
     <row r="34">
       <c r="A34" t="inlineStr">
         <is>
+          <t>_2007</t>
+        </is>
+      </c>
+      <c r="B34" t="inlineStr">
+        <is>
           <t>2007</t>
         </is>
       </c>
@@ -603,6 +758,11 @@
     <row r="35">
       <c r="A35" t="inlineStr">
         <is>
+          <t>_20072008</t>
+        </is>
+      </c>
+      <c r="B35" t="inlineStr">
+        <is>
           <t>2007/2008</t>
         </is>
       </c>
@@ -610,6 +770,11 @@
     <row r="36">
       <c r="A36" t="inlineStr">
         <is>
+          <t>_2008</t>
+        </is>
+      </c>
+      <c r="B36" t="inlineStr">
+        <is>
           <t>2008</t>
         </is>
       </c>
@@ -617,6 +782,11 @@
     <row r="37">
       <c r="A37" t="inlineStr">
         <is>
+          <t>_2009</t>
+        </is>
+      </c>
+      <c r="B37" t="inlineStr">
+        <is>
           <t>2009</t>
         </is>
       </c>
@@ -624,6 +794,11 @@
     <row r="38">
       <c r="A38" t="inlineStr">
         <is>
+          <t>_2009_2010</t>
+        </is>
+      </c>
+      <c r="B38" t="inlineStr">
+        <is>
           <t>2009/2010</t>
         </is>
       </c>
@@ -631,1323 +806,2488 @@
     <row r="39">
       <c r="A39" t="inlineStr">
         <is>
-          <t>2010</t>
+          <t>_20092010</t>
+        </is>
+      </c>
+      <c r="B39" t="inlineStr">
+        <is>
+          <t>2009/2010</t>
         </is>
       </c>
     </row>
     <row r="40">
       <c r="A40" t="inlineStr">
         <is>
-          <t>2011</t>
+          <t>_2010</t>
+        </is>
+      </c>
+      <c r="B40" t="inlineStr">
+        <is>
+          <t>2010</t>
         </is>
       </c>
     </row>
     <row r="41">
       <c r="A41" t="inlineStr">
         <is>
-          <t>2012</t>
+          <t>_2011</t>
+        </is>
+      </c>
+      <c r="B41" t="inlineStr">
+        <is>
+          <t>2011</t>
         </is>
       </c>
     </row>
     <row r="42">
       <c r="A42" t="inlineStr">
         <is>
-          <t>2013</t>
+          <t>_2012</t>
+        </is>
+      </c>
+      <c r="B42" t="inlineStr">
+        <is>
+          <t>2012</t>
         </is>
       </c>
     </row>
     <row r="43">
       <c r="A43" t="inlineStr">
         <is>
-          <t>2014</t>
+          <t>_2013</t>
+        </is>
+      </c>
+      <c r="B43" t="inlineStr">
+        <is>
+          <t>2013</t>
         </is>
       </c>
     </row>
     <row r="44">
       <c r="A44" t="inlineStr">
         <is>
-          <t>2015</t>
+          <t>_2014</t>
+        </is>
+      </c>
+      <c r="B44" t="inlineStr">
+        <is>
+          <t>2014</t>
         </is>
       </c>
     </row>
     <row r="45">
       <c r="A45" t="inlineStr">
         <is>
-          <t>2016</t>
+          <t>_2015</t>
+        </is>
+      </c>
+      <c r="B45" t="inlineStr">
+        <is>
+          <t>2015</t>
         </is>
       </c>
     </row>
     <row r="46">
       <c r="A46" t="inlineStr">
         <is>
-          <t>2017</t>
+          <t>_2016</t>
+        </is>
+      </c>
+      <c r="B46" t="inlineStr">
+        <is>
+          <t>2016</t>
         </is>
       </c>
     </row>
     <row r="47">
       <c r="A47" t="inlineStr">
         <is>
-          <t>2018</t>
+          <t>_2017</t>
+        </is>
+      </c>
+      <c r="B47" t="inlineStr">
+        <is>
+          <t>2017</t>
         </is>
       </c>
     </row>
     <row r="48">
       <c r="A48" t="inlineStr">
         <is>
-          <t>25-34</t>
+          <t>_2018</t>
+        </is>
+      </c>
+      <c r="B48" t="inlineStr">
+        <is>
+          <t>2018</t>
         </is>
       </c>
     </row>
     <row r="49">
       <c r="A49" t="inlineStr">
         <is>
-          <t>25 to 74</t>
+          <t>_20leastdeprived</t>
+        </is>
+      </c>
+      <c r="B49" t="inlineStr">
+        <is>
+          <t>20% least deprived</t>
         </is>
       </c>
     </row>
     <row r="50">
       <c r="A50" t="inlineStr">
         <is>
-          <t>3</t>
+          <t>_20mostdeprived</t>
+        </is>
+      </c>
+      <c r="B50" t="inlineStr">
+        <is>
+          <t>20% most deprived</t>
         </is>
       </c>
     </row>
     <row r="51">
       <c r="A51" t="inlineStr">
         <is>
-          <t>35 to 44</t>
+          <t>_2500130000</t>
+        </is>
+      </c>
+      <c r="B51" t="inlineStr">
+        <is>
+          <t>£25,001 to £30,000</t>
         </is>
       </c>
     </row>
     <row r="52">
       <c r="A52" t="inlineStr">
         <is>
-          <t>4</t>
+          <t>_2534</t>
+        </is>
+      </c>
+      <c r="B52" t="inlineStr">
+        <is>
+          <t>25-34</t>
         </is>
       </c>
     </row>
     <row r="53">
       <c r="A53" t="inlineStr">
         <is>
-          <t>40 to 59</t>
+          <t>_3</t>
+        </is>
+      </c>
+      <c r="B53" t="inlineStr">
+        <is>
+          <t>3</t>
         </is>
       </c>
     </row>
     <row r="54">
       <c r="A54" t="inlineStr">
         <is>
-          <t>40 to 64</t>
+          <t>_3000140000</t>
+        </is>
+      </c>
+      <c r="B54" t="inlineStr">
+        <is>
+          <t>£30,001 to £40,001</t>
         </is>
       </c>
     </row>
     <row r="55">
       <c r="A55" t="inlineStr">
         <is>
-          <t>45 to 59</t>
+          <t>_3544</t>
+        </is>
+      </c>
+      <c r="B55" t="inlineStr">
+        <is>
+          <t>35 to 44</t>
         </is>
       </c>
     </row>
     <row r="56">
       <c r="A56" t="inlineStr">
         <is>
-          <t>5 - 20% least deprived</t>
+          <t>_35to74</t>
+        </is>
+      </c>
+      <c r="B56" t="inlineStr">
+        <is>
+          <t>25 to 74</t>
         </is>
       </c>
     </row>
     <row r="57">
       <c r="A57" t="inlineStr">
         <is>
-          <t>6</t>
+          <t>_4</t>
+        </is>
+      </c>
+      <c r="B57" t="inlineStr">
+        <is>
+          <t>4</t>
         </is>
       </c>
     </row>
     <row r="58">
       <c r="A58" t="inlineStr">
         <is>
-          <t>60 plus</t>
+          <t>_4059</t>
+        </is>
+      </c>
+      <c r="B58" t="inlineStr">
+        <is>
+          <t>40 to 59</t>
         </is>
       </c>
     </row>
     <row r="59">
       <c r="A59" t="inlineStr">
         <is>
-          <t>60 to 74</t>
+          <t>_4064</t>
+        </is>
+      </c>
+      <c r="B59" t="inlineStr">
+        <is>
+          <t>40 to 64</t>
         </is>
       </c>
     </row>
     <row r="60">
       <c r="A60" t="inlineStr">
         <is>
-          <t>65 plus</t>
+          <t>_40to59</t>
+        </is>
+      </c>
+      <c r="B60" t="inlineStr">
+        <is>
+          <t>40 to 59</t>
         </is>
       </c>
     </row>
     <row r="61">
       <c r="A61" t="inlineStr">
         <is>
-          <t>75 plus</t>
+          <t>_4559</t>
+        </is>
+      </c>
+      <c r="B61" t="inlineStr">
+        <is>
+          <t>45 to 59</t>
         </is>
       </c>
     </row>
     <row r="62">
       <c r="A62" t="inlineStr">
         <is>
-          <t>Accessible rural</t>
+          <t>_520leastdeprived</t>
+        </is>
+      </c>
+      <c r="B62" t="inlineStr">
+        <is>
+          <t>5 - 20% least deprived</t>
         </is>
       </c>
     </row>
     <row r="63">
       <c r="A63" t="inlineStr">
         <is>
-          <t>Accessible small towns</t>
+          <t>_520LeastDeprived</t>
+        </is>
+      </c>
+      <c r="B63" t="inlineStr">
+        <is>
+          <t>5 - 20% least deprived</t>
         </is>
       </c>
     </row>
     <row r="64">
       <c r="A64" t="inlineStr">
         <is>
-          <t>Age</t>
+          <t>_5LeastDeprived</t>
+        </is>
+      </c>
+      <c r="B64" t="inlineStr">
+        <is>
+          <t>5 - 20% least deprived</t>
         </is>
       </c>
     </row>
     <row r="65">
       <c r="A65" t="inlineStr">
         <is>
-          <t>All</t>
+          <t>_6</t>
+        </is>
+      </c>
+      <c r="B65" t="inlineStr">
+        <is>
+          <t>6</t>
         </is>
       </c>
     </row>
     <row r="66">
       <c r="A66" t="inlineStr">
         <is>
-          <t>All adults</t>
+          <t>_60</t>
+        </is>
+      </c>
+      <c r="B66" t="inlineStr">
+        <is>
+          <t>60 plus</t>
         </is>
       </c>
     </row>
     <row r="67">
       <c r="A67" t="inlineStr">
         <is>
-          <t>annetinc</t>
+          <t>_600110000</t>
+        </is>
+      </c>
+      <c r="B67" t="inlineStr">
+        <is>
+          <t>£6,001 to £10,000</t>
         </is>
       </c>
     </row>
     <row r="68">
       <c r="A68" t="inlineStr">
         <is>
-          <t>Another way</t>
+          <t>_6074</t>
+        </is>
+      </c>
+      <c r="B68" t="inlineStr">
+        <is>
+          <t>60 to 74</t>
         </is>
       </c>
     </row>
     <row r="69">
       <c r="A69" t="inlineStr">
         <is>
-          <t>asp1</t>
+          <t>_65</t>
+        </is>
+      </c>
+      <c r="B69" t="inlineStr">
+        <is>
+          <t>65 plus</t>
         </is>
       </c>
     </row>
     <row r="70">
       <c r="A70" t="inlineStr">
         <is>
-          <t>asp1b</t>
+          <t>_75</t>
+        </is>
+      </c>
+      <c r="B70" t="inlineStr">
+        <is>
+          <t>75 plus</t>
         </is>
       </c>
     </row>
     <row r="71">
       <c r="A71" t="inlineStr">
         <is>
-          <t>asp2</t>
+          <t>_a.OwnerOccupier</t>
+        </is>
+      </c>
+      <c r="B71" t="inlineStr">
+        <is>
+          <t>Owner occupier</t>
         </is>
       </c>
     </row>
     <row r="72">
       <c r="A72" t="inlineStr">
         <is>
-          <t>ASP2</t>
+          <t>_Accessiblerural</t>
+        </is>
+      </c>
+      <c r="B72" t="inlineStr">
+        <is>
+          <t>Accessible rural</t>
         </is>
       </c>
     </row>
     <row r="73">
       <c r="A73" t="inlineStr">
         <is>
-          <t>At least once a week</t>
+          <t>_Accessiblesmalltowns</t>
+        </is>
+      </c>
+      <c r="B73" t="inlineStr">
+        <is>
+          <t>Accessible small towns</t>
         </is>
       </c>
     </row>
     <row r="74">
       <c r="A74" t="inlineStr">
         <is>
-          <t>Bad / very bad</t>
+          <t>_All</t>
+        </is>
+      </c>
+      <c r="B74" t="inlineStr">
+        <is>
+          <t>All</t>
         </is>
       </c>
     </row>
     <row r="75">
       <c r="A75" t="inlineStr">
         <is>
-          <t>Base</t>
+          <t>_All_1</t>
+        </is>
+      </c>
+      <c r="B75" t="inlineStr">
+        <is>
+          <t>All</t>
         </is>
       </c>
     </row>
     <row r="76">
       <c r="A76" t="inlineStr">
         <is>
-          <t>Base Discrimination</t>
+          <t>_All_2</t>
+        </is>
+      </c>
+      <c r="B76" t="inlineStr">
+        <is>
+          <t>All</t>
         </is>
       </c>
     </row>
     <row r="77">
       <c r="A77" t="inlineStr">
         <is>
-          <t>Base harassment</t>
+          <t>_All_Age</t>
+        </is>
+      </c>
+      <c r="B77" t="inlineStr">
+        <is>
+          <t>All</t>
         </is>
       </c>
     </row>
     <row r="78">
       <c r="A78" t="inlineStr">
         <is>
-          <t>c("1 - 20% most deprived", "1 - 20% most deprived")</t>
+          <t>_All_Gender</t>
+        </is>
+      </c>
+      <c r="B78" t="inlineStr">
+        <is>
+          <t>All</t>
         </is>
       </c>
     </row>
     <row r="79">
       <c r="A79" t="inlineStr">
         <is>
-          <t>Category</t>
+          <t>_AllAdults</t>
+        </is>
+      </c>
+      <c r="B79" t="inlineStr">
+        <is>
+          <t>All</t>
         </is>
       </c>
     </row>
     <row r="80">
       <c r="A80" t="inlineStr">
         <is>
-          <t>CLIMATE1</t>
+          <t>_AllAge</t>
+        </is>
+      </c>
+      <c r="B80" t="inlineStr">
+        <is>
+          <t>All</t>
         </is>
       </c>
     </row>
     <row r="81">
       <c r="A81" t="inlineStr">
         <is>
-          <t>CLIMATE2_A</t>
+          <t>_AllSIMD</t>
+        </is>
+      </c>
+      <c r="B81" t="inlineStr">
+        <is>
+          <t>All</t>
         </is>
       </c>
     </row>
     <row r="82">
       <c r="A82" t="inlineStr">
         <is>
-          <t>CLIMATE2_B</t>
+          <t>_Anotherway</t>
+        </is>
+      </c>
+      <c r="B82" t="inlineStr">
+        <is>
+          <t>Another way</t>
         </is>
       </c>
     </row>
     <row r="83">
       <c r="A83" t="inlineStr">
         <is>
-          <t>CLIMATE2_C</t>
+          <t>_Atleastonceaweek</t>
+        </is>
+      </c>
+      <c r="B83" t="inlineStr">
+        <is>
+          <t>At least once a week</t>
         </is>
       </c>
     </row>
     <row r="84">
       <c r="A84" t="inlineStr">
         <is>
-          <t>CLIMATE2_D</t>
+          <t>_b.Privaterent</t>
+        </is>
+      </c>
+      <c r="B84" t="inlineStr">
+        <is>
+          <t>Private rent</t>
         </is>
       </c>
     </row>
     <row r="85">
       <c r="A85" t="inlineStr">
         <is>
-          <t>commbel</t>
+          <t>_Base</t>
+        </is>
+      </c>
+      <c r="B85" t="inlineStr">
+        <is>
+          <t>Base</t>
         </is>
       </c>
     </row>
     <row r="86">
       <c r="A86" t="inlineStr">
         <is>
-          <t>Council</t>
+          <t>_Base_Discrim</t>
+        </is>
+      </c>
+      <c r="B86" t="inlineStr">
+        <is>
+          <t>Base Discrimination</t>
         </is>
       </c>
     </row>
     <row r="87">
       <c r="A87" t="inlineStr">
         <is>
-          <t>CultAny</t>
+          <t>_Base_Harass</t>
+        </is>
+      </c>
+      <c r="B87" t="inlineStr">
+        <is>
+          <t>Base harassment</t>
         </is>
       </c>
     </row>
     <row r="88">
       <c r="A88" t="inlineStr">
         <is>
-          <t>Degree / professional qualification</t>
+          <t>_c.SocialSector</t>
+        </is>
+      </c>
+      <c r="B88" t="inlineStr">
+        <is>
+          <t>Social sector</t>
         </is>
       </c>
     </row>
     <row r="89">
       <c r="A89" t="inlineStr">
         <is>
-          <t>description</t>
+          <t>_d.Other</t>
+        </is>
+      </c>
+      <c r="B89" t="inlineStr">
+        <is>
+          <t>Other</t>
         </is>
       </c>
     </row>
     <row r="90">
       <c r="A90" t="inlineStr">
         <is>
-          <t>Discrimination</t>
+          <t>_DegreeProfessionalQualification</t>
+        </is>
+      </c>
+      <c r="B90" t="inlineStr">
+        <is>
+          <t>Degree / professional qualification</t>
         </is>
       </c>
     </row>
     <row r="91">
       <c r="A91" t="inlineStr">
         <is>
-          <t>Don't know</t>
+          <t>_Discrim</t>
+        </is>
+      </c>
+      <c r="B91" t="inlineStr">
+        <is>
+          <t>Discrimination</t>
         </is>
       </c>
     </row>
     <row r="92">
       <c r="A92" t="inlineStr">
         <is>
-          <t>dyear</t>
+          <t>_Dontknow</t>
+        </is>
+      </c>
+      <c r="B92" t="inlineStr">
+        <is>
+          <t>Don't know</t>
         </is>
       </c>
     </row>
     <row r="93">
       <c r="A93" t="inlineStr">
         <is>
-          <t>Economic status</t>
+          <t>_DontKnow</t>
+        </is>
+      </c>
+      <c r="B93" t="inlineStr">
+        <is>
+          <t>Don't know</t>
         </is>
       </c>
     </row>
     <row r="94">
       <c r="A94" t="inlineStr">
         <is>
-          <t>Ethnicity</t>
+          <t>_Fair</t>
+        </is>
+      </c>
+      <c r="B94" t="inlineStr">
+        <is>
+          <t>Fair</t>
         </is>
       </c>
     </row>
     <row r="95">
       <c r="A95" t="inlineStr">
         <is>
-          <t>Experience</t>
+          <t>_Fairlystrongly</t>
+        </is>
+      </c>
+      <c r="B95" t="inlineStr">
+        <is>
+          <t>Fairly strongly</t>
         </is>
       </c>
     </row>
     <row r="96">
       <c r="A96" t="inlineStr">
         <is>
-          <t>Fair</t>
+          <t>_Female</t>
+        </is>
+      </c>
+      <c r="B96" t="inlineStr">
+        <is>
+          <t>Female</t>
         </is>
       </c>
     </row>
     <row r="97">
       <c r="A97" t="inlineStr">
         <is>
-          <t>Fairly strongly</t>
+          <t>_Harass</t>
+        </is>
+      </c>
+      <c r="B97" t="inlineStr">
+        <is>
+          <t>Harassment</t>
         </is>
       </c>
     </row>
     <row r="98">
       <c r="A98" t="inlineStr">
         <is>
-          <t>Female</t>
+          <t>_HigherAlevelOGradeStandardGrade</t>
+        </is>
+      </c>
+      <c r="B98" t="inlineStr">
+        <is>
+          <t>Higher/A level/O Grade/Standard Grade</t>
         </is>
       </c>
     </row>
     <row r="99">
       <c r="A99" t="inlineStr">
         <is>
-          <t>Gender</t>
+          <t>_HNCHNDorDegreeProf.Qual</t>
+        </is>
+      </c>
+      <c r="B99" t="inlineStr">
+        <is>
+          <t>HNC/HND/Degree/ Prof.Qualification</t>
         </is>
       </c>
     </row>
     <row r="100">
       <c r="A100" t="inlineStr">
         <is>
-          <t>Good / very good</t>
+          <t>_Identifiedinanotherway</t>
+        </is>
+      </c>
+      <c r="B100" t="inlineStr">
+        <is>
+          <t>Identified in another way</t>
         </is>
       </c>
     </row>
     <row r="101">
       <c r="A101" t="inlineStr">
         <is>
-          <t>greenfar13</t>
+          <t>_Inanotherway</t>
+        </is>
+      </c>
+      <c r="B101" t="inlineStr">
+        <is>
+          <t>In another way</t>
         </is>
       </c>
     </row>
     <row r="102">
       <c r="A102" t="inlineStr">
         <is>
-          <t>Harassment</t>
+          <t>_Inanotherway(ifyouwouldliketopl</t>
+        </is>
+      </c>
+      <c r="B102" t="inlineStr">
+        <is>
+          <t>In another way (part I can't read!)</t>
         </is>
       </c>
     </row>
     <row r="103">
       <c r="A103" t="inlineStr">
         <is>
-          <t>hc4</t>
+          <t>_Largeadult</t>
+        </is>
+      </c>
+      <c r="B103" t="inlineStr">
+        <is>
+          <t>Large adult</t>
         </is>
       </c>
     </row>
     <row r="104">
       <c r="A104" t="inlineStr">
         <is>
-          <t>hc6</t>
+          <t>_Largefamily</t>
+        </is>
+      </c>
+      <c r="B104" t="inlineStr">
+        <is>
+          <t>Large family</t>
         </is>
       </c>
     </row>
     <row r="105">
       <c r="A105" t="inlineStr">
         <is>
-          <t>hedqual8</t>
+          <t>_Larger</t>
+        </is>
+      </c>
+      <c r="B105" t="inlineStr">
+        <is>
+          <t>Larger</t>
         </is>
       </c>
     </row>
     <row r="106">
       <c r="A106" t="inlineStr">
         <is>
-          <t>Higher/A level/O Grade/Standard Grade</t>
+          <t>_Largeurbanareas</t>
+        </is>
+      </c>
+      <c r="B106" t="inlineStr">
+        <is>
+          <t>Large urban areas</t>
         </is>
       </c>
     </row>
     <row r="107">
       <c r="A107" t="inlineStr">
         <is>
-          <t>hihage</t>
+          <t>_Longtermcondition_1</t>
+        </is>
+      </c>
+      <c r="B107" t="inlineStr">
+        <is>
+          <t>Yes long-term condition</t>
         </is>
       </c>
     </row>
     <row r="108">
       <c r="A108" t="inlineStr">
         <is>
-          <t>HNC/HND/Degree/ Prof.Qualification</t>
+          <t>_Longtermcondition_2</t>
+        </is>
+      </c>
+      <c r="B108" t="inlineStr">
+        <is>
+          <t>Yes ('excluding permanently sick or disabled')</t>
         </is>
       </c>
     </row>
     <row r="109">
       <c r="A109" t="inlineStr">
         <is>
-          <t>Household type</t>
+          <t>_Male</t>
+        </is>
+      </c>
+      <c r="B109" t="inlineStr">
+        <is>
+          <t>Male</t>
         </is>
       </c>
     </row>
     <row r="110">
       <c r="A110" t="inlineStr">
         <is>
-          <t>Identified in another way</t>
+          <t>_ManBoy</t>
+        </is>
+      </c>
+      <c r="B110" t="inlineStr">
+        <is>
+          <t>Man / Boy</t>
         </is>
       </c>
     </row>
     <row r="111">
       <c r="A111" t="inlineStr">
         <is>
-          <t>In another way</t>
+          <t>_NAME_</t>
         </is>
       </c>
     </row>
     <row r="112">
       <c r="A112" t="inlineStr">
         <is>
-          <t>In another way (part I can't read!)</t>
+          <t>_Neitheragreenordisagree</t>
+        </is>
+      </c>
+      <c r="B112" t="inlineStr">
+        <is>
+          <t>Neither agree nor disagree</t>
         </is>
       </c>
     </row>
     <row r="113">
       <c r="A113" t="inlineStr">
         <is>
-          <t>LABEL</t>
+          <t>_No</t>
+        </is>
+      </c>
+      <c r="B113" t="inlineStr">
+        <is>
+          <t>No</t>
         </is>
       </c>
     </row>
     <row r="114">
       <c r="A114" t="inlineStr">
         <is>
-          <t>Large adult</t>
+          <t>_No_Disc</t>
+        </is>
+      </c>
+      <c r="B114" t="inlineStr">
+        <is>
+          <t>No Discrimination</t>
         </is>
       </c>
     </row>
     <row r="115">
       <c r="A115" t="inlineStr">
         <is>
-          <t>Large family</t>
+          <t>_No_Discrim</t>
+        </is>
+      </c>
+      <c r="B115" t="inlineStr">
+        <is>
+          <t>No Discrimination</t>
         </is>
       </c>
     </row>
     <row r="116">
       <c r="A116" t="inlineStr">
         <is>
-          <t>Large urban areas</t>
+          <t>_No_Harass</t>
+        </is>
+      </c>
+      <c r="B116" t="inlineStr">
+        <is>
+          <t>No Harassment</t>
         </is>
       </c>
     </row>
     <row r="117">
       <c r="A117" t="inlineStr">
         <is>
-          <t>Larger</t>
+          <t>_Nochildren</t>
+        </is>
+      </c>
+      <c r="B117" t="inlineStr">
+        <is>
+          <t>No children</t>
         </is>
       </c>
     </row>
     <row r="118">
       <c r="A118" t="inlineStr">
         <is>
-          <t>Local Authority</t>
+          <t>_nolongtermcondition_1</t>
+        </is>
+      </c>
+      <c r="B118" t="inlineStr">
+        <is>
+          <t>No long-term condition</t>
         </is>
       </c>
     </row>
     <row r="119">
       <c r="A119" t="inlineStr">
         <is>
-          <t>Long-term physical or mental health condition</t>
+          <t>_nolongtermcondition_2</t>
+        </is>
+      </c>
+      <c r="B119" t="inlineStr">
+        <is>
+          <t>No ('excluding permanently sick or disabled')</t>
         </is>
       </c>
     </row>
     <row r="120">
       <c r="A120" t="inlineStr">
         <is>
-          <t>Male</t>
+          <t>_None</t>
+        </is>
+      </c>
+      <c r="B120" t="inlineStr">
+        <is>
+          <t>None</t>
         </is>
       </c>
     </row>
     <row r="121">
       <c r="A121" t="inlineStr">
         <is>
-          <t>Man / Boy</t>
+          <t>_Noqualifications</t>
+        </is>
+      </c>
+      <c r="B121" t="inlineStr">
+        <is>
+          <t>No qualifications</t>
         </is>
       </c>
     </row>
     <row r="122">
       <c r="A122" t="inlineStr">
         <is>
-          <t>Marital status</t>
+          <t>_Notatallstrongly</t>
+        </is>
+      </c>
+      <c r="B122" t="inlineStr">
+        <is>
+          <t>Not at all strongly</t>
         </is>
       </c>
     </row>
     <row r="123">
       <c r="A123" t="inlineStr">
         <is>
-          <t>Neither agree nor disagree</t>
+          <t>_Notverystrongly</t>
+        </is>
+      </c>
+      <c r="B123" t="inlineStr">
+        <is>
+          <t>Not very strongly</t>
         </is>
       </c>
     </row>
     <row r="124">
       <c r="A124" t="inlineStr">
         <is>
-          <t>net1</t>
+          <t>_O_StandHigherAlevelorequivalent</t>
+        </is>
+      </c>
+      <c r="B124" t="inlineStr">
+        <is>
+          <t>O grade/Standard grade/Higher/A level/Equivalent</t>
         </is>
       </c>
     </row>
     <row r="125">
       <c r="A125" t="inlineStr">
         <is>
-          <t>NET6C2018</t>
+          <t>_Oldersmaller</t>
+        </is>
+      </c>
+      <c r="B125" t="inlineStr">
+        <is>
+          <t>Older smaller</t>
         </is>
       </c>
     </row>
     <row r="126">
       <c r="A126" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>_onceamonthandwithinyear</t>
+        </is>
+      </c>
+      <c r="B126" t="inlineStr">
+        <is>
+          <t>Once a month and within year</t>
         </is>
       </c>
     </row>
     <row r="127">
       <c r="A127" t="inlineStr">
         <is>
-          <t>No ('excluding permanently sick or disabled')</t>
+          <t>_onceaweekbutatleastonceamonth</t>
+        </is>
+      </c>
+      <c r="B127" t="inlineStr">
+        <is>
+          <t>Once a week but at least once a month</t>
         </is>
       </c>
     </row>
     <row r="128">
       <c r="A128" t="inlineStr">
         <is>
-          <t>No children</t>
+          <t>_Other</t>
+        </is>
+      </c>
+      <c r="B128" t="inlineStr">
+        <is>
+          <t>Other</t>
         </is>
       </c>
     </row>
     <row r="129">
       <c r="A129" t="inlineStr">
         <is>
-          <t>No Discrimination</t>
+          <t>_Otherqualification</t>
+        </is>
+      </c>
+      <c r="B129" t="inlineStr">
+        <is>
+          <t>Other qualification</t>
         </is>
       </c>
     </row>
     <row r="130">
       <c r="A130" t="inlineStr">
         <is>
-          <t>No Harassment</t>
+          <t>_Otherurbanareas</t>
+        </is>
+      </c>
+      <c r="B130" t="inlineStr">
+        <is>
+          <t>Other urban areas</t>
         </is>
       </c>
     </row>
     <row r="131">
       <c r="A131" t="inlineStr">
         <is>
-          <t>No long-term condition</t>
+          <t>_Over30000</t>
+        </is>
+      </c>
+      <c r="B131" t="inlineStr">
+        <is>
+          <t>Over £30,000</t>
         </is>
       </c>
     </row>
     <row r="132">
       <c r="A132" t="inlineStr">
         <is>
-          <t>No qualifications</t>
+          <t>_Over40000</t>
+        </is>
+      </c>
+      <c r="B132" t="inlineStr">
+        <is>
+          <t>Over £40,000</t>
         </is>
       </c>
     </row>
     <row r="133">
       <c r="A133" t="inlineStr">
         <is>
-          <t>None</t>
+          <t>_Ownbuyownhome</t>
+        </is>
+      </c>
+      <c r="B133" t="inlineStr">
+        <is>
+          <t>Own / buy own home</t>
         </is>
       </c>
     </row>
     <row r="134">
       <c r="A134" t="inlineStr">
         <is>
-          <t>Not at all strongly</t>
+          <t>_Owned</t>
+        </is>
+      </c>
+      <c r="B134" t="inlineStr">
+        <is>
+          <t>Owned</t>
         </is>
       </c>
     </row>
     <row r="135">
       <c r="A135" t="inlineStr">
         <is>
-          <t>Not very strongly</t>
+          <t>_Owneroccupied</t>
+        </is>
+      </c>
+      <c r="B135" t="inlineStr">
+        <is>
+          <t>Owner occupied</t>
         </is>
       </c>
     </row>
     <row r="136">
       <c r="A136" t="inlineStr">
         <is>
-          <t>numbhh</t>
+          <t>_Permanentlyretiredfromwork</t>
+        </is>
+      </c>
+      <c r="B136" t="inlineStr">
+        <is>
+          <t>Permanently retired from work</t>
         </is>
       </c>
     </row>
     <row r="137">
       <c r="A137" t="inlineStr">
         <is>
-          <t>numcars</t>
+          <t>_Privaterented</t>
+        </is>
+      </c>
+      <c r="B137" t="inlineStr">
+        <is>
+          <t>Private rented</t>
         </is>
       </c>
     </row>
     <row r="138">
       <c r="A138" t="inlineStr">
         <is>
-          <t>O grade/Standard grade/Higher/A level/Equivalent</t>
+          <t>_PrivateRented</t>
+        </is>
+      </c>
+      <c r="B138" t="inlineStr">
+        <is>
+          <t>Private rented</t>
         </is>
       </c>
     </row>
     <row r="139">
       <c r="A139" t="inlineStr">
         <is>
-          <t>Older smaller</t>
+          <t>_Qualificationsnotknown</t>
+        </is>
+      </c>
+      <c r="B139" t="inlineStr">
+        <is>
+          <t>Qualifications not known</t>
         </is>
       </c>
     </row>
     <row r="140">
       <c r="A140" t="inlineStr">
         <is>
-          <t>Once a month and within year</t>
+          <t>_Refusal</t>
+        </is>
+      </c>
+      <c r="B140" t="inlineStr">
+        <is>
+          <t>Refusal</t>
         </is>
       </c>
     </row>
     <row r="141">
       <c r="A141" t="inlineStr">
         <is>
-          <t>Once a week but at least once a month</t>
+          <t>_Refused</t>
+        </is>
+      </c>
+      <c r="B141" t="inlineStr">
+        <is>
+          <t>Refused</t>
         </is>
       </c>
     </row>
     <row r="142">
       <c r="A142" t="inlineStr">
         <is>
-          <t>Other</t>
+          <t>_Refused(spontaneous)</t>
+        </is>
+      </c>
+      <c r="B142" t="inlineStr">
+        <is>
+          <t>Refused</t>
         </is>
       </c>
     </row>
     <row r="143">
       <c r="A143" t="inlineStr">
         <is>
-          <t>Other qualification</t>
+          <t>_Remoterural</t>
+        </is>
+      </c>
+      <c r="B143" t="inlineStr">
+        <is>
+          <t>Remote rural</t>
         </is>
       </c>
     </row>
     <row r="144">
       <c r="A144" t="inlineStr">
         <is>
-          <t>Other urban areas</t>
+          <t>_Remotesmalltowns</t>
+        </is>
+      </c>
+      <c r="B144" t="inlineStr">
+        <is>
+          <t>Remote small towns</t>
         </is>
       </c>
     </row>
     <row r="145">
       <c r="A145" t="inlineStr">
         <is>
-          <t>outdoor</t>
+          <t>_Rentprivatelandlord</t>
+        </is>
+      </c>
+      <c r="B145" t="inlineStr">
+        <is>
+          <t>Rent - private landlord</t>
         </is>
       </c>
     </row>
     <row r="146">
       <c r="A146" t="inlineStr">
         <is>
-          <t>Over £30,000</t>
+          <t>_Rentsocialhousing</t>
+        </is>
+      </c>
+      <c r="B146" t="inlineStr">
+        <is>
+          <t>Rent - social housing</t>
         </is>
       </c>
     </row>
     <row r="147">
       <c r="A147" t="inlineStr">
         <is>
-          <t>Over £40,000</t>
+          <t>_Ruralareas</t>
+        </is>
+      </c>
+      <c r="B147" t="inlineStr">
+        <is>
+          <t>Rural areas</t>
         </is>
       </c>
     </row>
     <row r="148">
       <c r="A148" t="inlineStr">
         <is>
-          <t>Own / buy own home</t>
+          <t>_RuralAreas</t>
+        </is>
+      </c>
+      <c r="B148" t="inlineStr">
+        <is>
+          <t>Rural areas</t>
         </is>
       </c>
     </row>
     <row r="149">
       <c r="A149" t="inlineStr">
         <is>
-          <t>Owned</t>
+          <t>_Samesizeascurrent</t>
+        </is>
+      </c>
+      <c r="B149" t="inlineStr">
+        <is>
+          <t>Same size as current</t>
         </is>
       </c>
     </row>
     <row r="150">
       <c r="A150" t="inlineStr">
         <is>
-          <t>Owner occupied</t>
+          <t>_Selfemployedfullparttimeemploym</t>
+        </is>
+      </c>
+      <c r="B150" t="inlineStr">
+        <is>
+          <t>Self employed/full-/part-/time employment</t>
         </is>
       </c>
     </row>
     <row r="151">
       <c r="A151" t="inlineStr">
         <is>
-          <t>Owner occupier</t>
+          <t>_Singleadult</t>
+        </is>
+      </c>
+      <c r="B151" t="inlineStr">
+        <is>
+          <t>Single adult</t>
         </is>
       </c>
     </row>
     <row r="152">
       <c r="A152" t="inlineStr">
         <is>
-          <t>pa1</t>
+          <t>_Singleparent</t>
+        </is>
+      </c>
+      <c r="B152" t="inlineStr">
+        <is>
+          <t>Single parent</t>
         </is>
       </c>
     </row>
     <row r="153">
       <c r="A153" t="inlineStr">
         <is>
-          <t>Perception</t>
+          <t>_Singlepensioner</t>
+        </is>
+      </c>
+      <c r="B153" t="inlineStr">
+        <is>
+          <t>Single pensioner</t>
         </is>
       </c>
     </row>
     <row r="154">
       <c r="A154" t="inlineStr">
         <is>
-          <t>Permanently retired from work</t>
+          <t>_Smalladult</t>
+        </is>
+      </c>
+      <c r="B154" t="inlineStr">
+        <is>
+          <t>Small adult</t>
         </is>
       </c>
     </row>
     <row r="155">
       <c r="A155" t="inlineStr">
         <is>
-          <t>previoustenure</t>
+          <t>_Smaller</t>
+        </is>
+      </c>
+      <c r="B155" t="inlineStr">
+        <is>
+          <t>Smaller</t>
         </is>
       </c>
     </row>
     <row r="156">
       <c r="A156" t="inlineStr">
         <is>
-          <t>Private rent</t>
+          <t>_Smallfamily</t>
+        </is>
+      </c>
+      <c r="B156" t="inlineStr">
+        <is>
+          <t>Small family</t>
         </is>
       </c>
     </row>
     <row r="157">
       <c r="A157" t="inlineStr">
         <is>
-          <t>Private rented</t>
+          <t>_Socialrented</t>
+        </is>
+      </c>
+      <c r="B157" t="inlineStr">
+        <is>
+          <t>Social rented</t>
         </is>
       </c>
     </row>
     <row r="158">
       <c r="A158" t="inlineStr">
         <is>
-          <t>Property type</t>
+          <t>_SocialRented</t>
+        </is>
+      </c>
+      <c r="B158" t="inlineStr">
+        <is>
+          <t>Social rented</t>
         </is>
       </c>
     </row>
     <row r="159">
       <c r="A159" t="inlineStr">
         <is>
-          <t>Qualifications not known</t>
+          <t>_Stronglyagree</t>
+        </is>
+      </c>
+      <c r="B159" t="inlineStr">
+        <is>
+          <t>Strongly agree</t>
         </is>
       </c>
     </row>
     <row r="160">
       <c r="A160" t="inlineStr">
         <is>
-          <t>ra1</t>
+          <t>_Stronglydisagree</t>
+        </is>
+      </c>
+      <c r="B160" t="inlineStr">
+        <is>
+          <t>Strongly disagree</t>
         </is>
       </c>
     </row>
     <row r="161">
       <c r="A161" t="inlineStr">
         <is>
-          <t>ra15_2017</t>
+          <t>_Tendtoagree</t>
+        </is>
+      </c>
+      <c r="B161" t="inlineStr">
+        <is>
+          <t>Tend to agree</t>
         </is>
       </c>
     </row>
     <row r="162">
       <c r="A162" t="inlineStr">
         <is>
-          <t>ra15a</t>
+          <t>_Tendtodisagree</t>
+        </is>
+      </c>
+      <c r="B162" t="inlineStr">
+        <is>
+          <t>Tend to disagree</t>
         </is>
       </c>
     </row>
     <row r="163">
       <c r="A163" t="inlineStr">
         <is>
-          <t>ra15b</t>
+          <t>_Tojoinanexistingfamilyorhouseho</t>
+        </is>
+      </c>
+      <c r="B163" t="inlineStr">
+        <is>
+          <t>To join an existing family or household</t>
         </is>
       </c>
     </row>
     <row r="164">
       <c r="A164" t="inlineStr">
         <is>
-          <t>ra15c</t>
+          <t>_Tooccupytheentireproperty</t>
+        </is>
+      </c>
+      <c r="B164" t="inlineStr">
+        <is>
+          <t>To occupy the entire property</t>
         </is>
       </c>
     </row>
     <row r="165">
       <c r="A165" t="inlineStr">
         <is>
-          <t>rahl2</t>
+          <t>_Upto15000</t>
+        </is>
+      </c>
+      <c r="B165" t="inlineStr">
+        <is>
+          <t>Up to £15,000</t>
         </is>
       </c>
     </row>
     <row r="166">
       <c r="A166" t="inlineStr">
         <is>
-          <t>rb1</t>
+          <t>_Urbanareas</t>
+        </is>
+      </c>
+      <c r="B166" t="inlineStr">
+        <is>
+          <t>Urban areas</t>
         </is>
       </c>
     </row>
     <row r="167">
       <c r="A167" t="inlineStr">
         <is>
-          <t>Refusal</t>
+          <t>_UrbanAreas</t>
+        </is>
+      </c>
+      <c r="B167" t="inlineStr">
+        <is>
+          <t>Urban areas</t>
         </is>
       </c>
     </row>
     <row r="168">
       <c r="A168" t="inlineStr">
         <is>
-          <t>Refused</t>
+          <t>_VeryBadBad</t>
+        </is>
+      </c>
+      <c r="B168" t="inlineStr">
+        <is>
+          <t>Bad / very bad</t>
         </is>
       </c>
     </row>
     <row r="169">
       <c r="A169" t="inlineStr">
         <is>
-          <t>Religious and ethnic belonging</t>
+          <t>_VeryGoodGood</t>
+        </is>
+      </c>
+      <c r="B169" t="inlineStr">
+        <is>
+          <t>Good / very good</t>
         </is>
       </c>
     </row>
     <row r="170">
       <c r="A170" t="inlineStr">
         <is>
-          <t>Remote rural</t>
+          <t>_Verystrongly</t>
+        </is>
+      </c>
+      <c r="B170" t="inlineStr">
+        <is>
+          <t>Very strongly</t>
         </is>
       </c>
     </row>
     <row r="171">
       <c r="A171" t="inlineStr">
         <is>
-          <t>Remote small towns</t>
+          <t>_WomanGirl</t>
+        </is>
+      </c>
+      <c r="B171" t="inlineStr">
+        <is>
+          <t>Woman / Girl</t>
         </is>
       </c>
     </row>
     <row r="172">
       <c r="A172" t="inlineStr">
         <is>
-          <t>Rent - private landlord</t>
+          <t>_Yes</t>
+        </is>
+      </c>
+      <c r="B172" t="inlineStr">
+        <is>
+          <t>Yes</t>
         </is>
       </c>
     </row>
     <row r="173">
       <c r="A173" t="inlineStr">
         <is>
-          <t>Rent - social housing</t>
+          <t>_Yes_Disc</t>
+        </is>
+      </c>
+      <c r="B173" t="inlineStr">
+        <is>
+          <t>Yes Discrimination</t>
         </is>
       </c>
     </row>
     <row r="174">
       <c r="A174" t="inlineStr">
         <is>
-          <t>RESIL1</t>
+          <t>_Yes_Discrim</t>
+        </is>
+      </c>
+      <c r="B174" t="inlineStr">
+        <is>
+          <t>Yes Discrimination</t>
         </is>
       </c>
     </row>
     <row r="175">
       <c r="A175" t="inlineStr">
         <is>
-          <t>response</t>
+          <t>_Yes_Harass</t>
+        </is>
+      </c>
+      <c r="B175" t="inlineStr">
+        <is>
+          <t>Yes Harassment</t>
         </is>
       </c>
     </row>
     <row r="176">
       <c r="A176" t="inlineStr">
         <is>
-          <t>RESPONSE</t>
+          <t>_Yesalittle</t>
+        </is>
+      </c>
+      <c r="B176" t="inlineStr">
+        <is>
+          <t>Yes a little</t>
         </is>
       </c>
     </row>
     <row r="177">
       <c r="A177" t="inlineStr">
         <is>
-          <t>Rural areas</t>
+          <t>_Yesalot</t>
+        </is>
+      </c>
+      <c r="B177" t="inlineStr">
+        <is>
+          <t>Yes a lot</t>
         </is>
       </c>
     </row>
     <row r="178">
       <c r="A178" t="inlineStr">
         <is>
-          <t>Same size as current</t>
+          <t>_Yesbutnoreducedcapacity</t>
+        </is>
+      </c>
+      <c r="B178" t="inlineStr">
+        <is>
+          <t>Yes but no reduced capacity</t>
         </is>
       </c>
     </row>
     <row r="179">
       <c r="A179" t="inlineStr">
         <is>
-          <t>Self employed/full-/part-/time employment</t>
+          <t>_Yeshavechildren</t>
+        </is>
+      </c>
+      <c r="B179" t="inlineStr">
+        <is>
+          <t>Yes have children</t>
         </is>
       </c>
     </row>
     <row r="180">
       <c r="A180" t="inlineStr">
         <is>
-          <t>Sexual orientation</t>
+          <t>1999</t>
         </is>
       </c>
     </row>
     <row r="181">
       <c r="A181" t="inlineStr">
         <is>
-          <t>SIMD quintile</t>
+          <t>2000</t>
         </is>
       </c>
     </row>
     <row r="182">
       <c r="A182" t="inlineStr">
         <is>
-          <t>SIMD Quintiles</t>
+          <t>2001</t>
         </is>
       </c>
     </row>
     <row r="183">
       <c r="A183" t="inlineStr">
         <is>
-          <t>Single adult</t>
+          <t>2002</t>
         </is>
       </c>
     </row>
     <row r="184">
       <c r="A184" t="inlineStr">
         <is>
-          <t>Single parent</t>
+          <t>2003</t>
         </is>
       </c>
     </row>
     <row r="185">
       <c r="A185" t="inlineStr">
         <is>
-          <t>Single pensioner</t>
+          <t>2004</t>
         </is>
       </c>
     </row>
     <row r="186">
       <c r="A186" t="inlineStr">
         <is>
-          <t>Small adult</t>
+          <t>2005</t>
         </is>
       </c>
     </row>
     <row r="187">
       <c r="A187" t="inlineStr">
         <is>
-          <t>Small family</t>
+          <t>2006</t>
         </is>
       </c>
     </row>
     <row r="188">
       <c r="A188" t="inlineStr">
         <is>
-          <t>Smaller</t>
+          <t>2007</t>
         </is>
       </c>
     </row>
     <row r="189">
       <c r="A189" t="inlineStr">
         <is>
-          <t>Social rented</t>
+          <t>2008</t>
         </is>
       </c>
     </row>
     <row r="190">
       <c r="A190" t="inlineStr">
         <is>
-          <t>Social sector</t>
+          <t>2009</t>
         </is>
       </c>
     </row>
     <row r="191">
       <c r="A191" t="inlineStr">
         <is>
-          <t>social1</t>
+          <t>2010</t>
         </is>
       </c>
     </row>
     <row r="192">
       <c r="A192" t="inlineStr">
         <is>
-          <t>social2</t>
+          <t>2011</t>
         </is>
       </c>
     </row>
     <row r="193">
       <c r="A193" t="inlineStr">
         <is>
-          <t>Status</t>
+          <t>2012</t>
         </is>
       </c>
     </row>
     <row r="194">
       <c r="A194" t="inlineStr">
         <is>
-          <t>Strongly agree</t>
+          <t>2013</t>
         </is>
       </c>
     </row>
     <row r="195">
       <c r="A195" t="inlineStr">
         <is>
-          <t>Strongly disagree</t>
+          <t>2014</t>
         </is>
       </c>
     </row>
     <row r="196">
       <c r="A196" t="inlineStr">
         <is>
-          <t>Tend to agree</t>
+          <t>2015</t>
         </is>
       </c>
     </row>
     <row r="197">
       <c r="A197" t="inlineStr">
         <is>
-          <t>Tend to disagree</t>
+          <t>2016</t>
         </is>
       </c>
     </row>
     <row r="198">
       <c r="A198" t="inlineStr">
         <is>
-          <t>Tenure</t>
+          <t>2017</t>
         </is>
       </c>
     </row>
     <row r="199">
       <c r="A199" t="inlineStr">
         <is>
-          <t>tenurealt</t>
+          <t>2018</t>
         </is>
       </c>
     </row>
     <row r="200">
       <c r="A200" t="inlineStr">
         <is>
-          <t>To join an existing family or household</t>
+          <t>age</t>
+        </is>
+      </c>
+      <c r="B200" t="inlineStr">
+        <is>
+          <t>Age</t>
         </is>
       </c>
     </row>
     <row r="201">
       <c r="A201" t="inlineStr">
         <is>
-          <t>To occupy the entire property</t>
+          <t>Alladults</t>
+        </is>
+      </c>
+      <c r="B201" t="inlineStr">
+        <is>
+          <t>All adults</t>
         </is>
       </c>
     </row>
     <row r="202">
       <c r="A202" t="inlineStr">
         <is>
-          <t>tothinc</t>
+          <t>annetinc</t>
         </is>
       </c>
     </row>
     <row r="203">
       <c r="A203" t="inlineStr">
         <is>
-          <t>Up to £15,000</t>
+          <t>asp1</t>
         </is>
       </c>
     </row>
     <row r="204">
       <c r="A204" t="inlineStr">
         <is>
-          <t>Up to £6,000</t>
+          <t>asp1b</t>
         </is>
       </c>
     </row>
     <row r="205">
       <c r="A205" t="inlineStr">
         <is>
-          <t>Urban areas</t>
+          <t>asp2</t>
         </is>
       </c>
     </row>
     <row r="206">
       <c r="A206" t="inlineStr">
         <is>
-          <t>Urban/rural classification</t>
+          <t>ASP2</t>
         </is>
       </c>
     </row>
     <row r="207">
       <c r="A207" t="inlineStr">
         <is>
-          <t>var</t>
+          <t>base</t>
+        </is>
+      </c>
+      <c r="B207" t="inlineStr">
+        <is>
+          <t>Base</t>
         </is>
       </c>
     </row>
     <row r="208">
       <c r="A208" t="inlineStr">
         <is>
-          <t>Very strongly</t>
+          <t>Category</t>
         </is>
       </c>
     </row>
     <row r="209">
       <c r="A209" t="inlineStr">
         <is>
-          <t>vol32018</t>
+          <t>CLIMATE1</t>
         </is>
       </c>
     </row>
     <row r="210">
       <c r="A210" t="inlineStr">
         <is>
-          <t>vol42018</t>
+          <t>CLIMATE2_A</t>
         </is>
       </c>
     </row>
     <row r="211">
       <c r="A211" t="inlineStr">
         <is>
-          <t>volinform</t>
+          <t>CLIMATE2_B</t>
         </is>
       </c>
     </row>
     <row r="212">
       <c r="A212" t="inlineStr">
         <is>
-          <t>voliv2</t>
+          <t>CLIMATE2_C</t>
         </is>
       </c>
     </row>
     <row r="213">
       <c r="A213" t="inlineStr">
         <is>
-          <t>voliv3</t>
+          <t>CLIMATE2_D</t>
         </is>
       </c>
     </row>
     <row r="214">
       <c r="A214" t="inlineStr">
         <is>
-          <t>voluntee</t>
+          <t>commbel</t>
         </is>
       </c>
     </row>
     <row r="215">
       <c r="A215" t="inlineStr">
         <is>
-          <t>Woman / Girl</t>
+          <t>council</t>
+        </is>
+      </c>
+      <c r="B215" t="inlineStr">
+        <is>
+          <t>Council</t>
         </is>
       </c>
     </row>
     <row r="216">
       <c r="A216" t="inlineStr">
         <is>
-          <t>Working age adults</t>
+          <t>CultAny</t>
         </is>
       </c>
     </row>
     <row r="217">
       <c r="A217" t="inlineStr">
         <is>
-          <t>working_adults</t>
+          <t>description</t>
         </is>
       </c>
     </row>
     <row r="218">
       <c r="A218" t="inlineStr">
         <is>
-          <t>Year</t>
+          <t>dyear</t>
         </is>
       </c>
     </row>
     <row r="219">
       <c r="A219" t="inlineStr">
         <is>
-          <t>Yes</t>
+          <t>Experience</t>
         </is>
       </c>
     </row>
     <row r="220">
       <c r="A220" t="inlineStr">
         <is>
-          <t>Yes ('excluding permanently sick or disabled')</t>
+          <t>Gender</t>
         </is>
       </c>
     </row>
     <row r="221">
       <c r="A221" t="inlineStr">
         <is>
-          <t>Yes a little</t>
+          <t>greenfar13</t>
         </is>
       </c>
     </row>
     <row r="222">
       <c r="A222" t="inlineStr">
         <is>
-          <t>Yes a lot</t>
+          <t>ha5</t>
+        </is>
+      </c>
+      <c r="B222" t="inlineStr">
+        <is>
+          <t>Age</t>
         </is>
       </c>
     </row>
     <row r="223">
       <c r="A223" t="inlineStr">
         <is>
-          <t>Yes but no reduced capacity</t>
+          <t>ha6</t>
+        </is>
+      </c>
+      <c r="B223" t="inlineStr">
+        <is>
+          <t>Gender</t>
         </is>
       </c>
     </row>
     <row r="224">
       <c r="A224" t="inlineStr">
         <is>
-          <t>Yes Discrimination</t>
+          <t>ha7</t>
+        </is>
+      </c>
+      <c r="B224" t="inlineStr">
+        <is>
+          <t>Economic status</t>
         </is>
       </c>
     </row>
     <row r="225">
       <c r="A225" t="inlineStr">
         <is>
-          <t>Yes Harassment</t>
+          <t>hb1</t>
+        </is>
+      </c>
+      <c r="B225" t="inlineStr">
+        <is>
+          <t>Property type</t>
         </is>
       </c>
     </row>
     <row r="226">
       <c r="A226" t="inlineStr">
         <is>
-          <t>Yes have children</t>
+          <t>hc4</t>
         </is>
       </c>
     </row>
     <row r="227">
       <c r="A227" t="inlineStr">
         <is>
-          <t>Yes long-term condition</t>
+          <t>hc6</t>
+        </is>
+      </c>
+    </row>
+    <row r="228">
+      <c r="A228" t="inlineStr">
+        <is>
+          <t>hedqual8</t>
+        </is>
+      </c>
+    </row>
+    <row r="229">
+      <c r="A229" t="inlineStr">
+        <is>
+          <t>hf1an</t>
+        </is>
+      </c>
+      <c r="B229" t="inlineStr">
+        <is>
+          <t>Long-term physical or mental health condition</t>
+        </is>
+      </c>
+    </row>
+    <row r="230">
+      <c r="A230" t="inlineStr">
+        <is>
+          <t>hhtype</t>
+        </is>
+      </c>
+      <c r="B230" t="inlineStr">
+        <is>
+          <t>Household type</t>
+        </is>
+      </c>
+    </row>
+    <row r="231">
+      <c r="A231" t="inlineStr">
+        <is>
+          <t>hhtype_new</t>
+        </is>
+      </c>
+      <c r="B231" t="inlineStr">
+        <is>
+          <t>Household type</t>
+        </is>
+      </c>
+    </row>
+    <row r="232">
+      <c r="A232" t="inlineStr">
+        <is>
+          <t>hihage</t>
+        </is>
+      </c>
+    </row>
+    <row r="233">
+      <c r="A233" t="inlineStr">
+        <is>
+          <t>hk2</t>
+        </is>
+      </c>
+      <c r="B233" t="inlineStr">
+        <is>
+          <t>Status</t>
+        </is>
+      </c>
+    </row>
+    <row r="234">
+      <c r="A234" t="inlineStr">
+        <is>
+          <t>LABEL</t>
+        </is>
+      </c>
+    </row>
+    <row r="235">
+      <c r="A235" t="inlineStr">
+        <is>
+          <t>Local Authority</t>
+        </is>
+      </c>
+    </row>
+    <row r="236">
+      <c r="A236" t="inlineStr">
+        <is>
+          <t>md12quin</t>
+        </is>
+      </c>
+      <c r="B236" t="inlineStr">
+        <is>
+          <t>SIMD quintile</t>
+        </is>
+      </c>
+    </row>
+    <row r="237">
+      <c r="A237" t="inlineStr">
+        <is>
+          <t>md16quin</t>
+        </is>
+      </c>
+      <c r="B237" t="inlineStr">
+        <is>
+          <t>SIMD quintile</t>
+        </is>
+      </c>
+    </row>
+    <row r="238">
+      <c r="A238" t="inlineStr">
+        <is>
+          <t>net1</t>
+        </is>
+      </c>
+    </row>
+    <row r="239">
+      <c r="A239" t="inlineStr">
+        <is>
+          <t>NET6C2018</t>
+        </is>
+      </c>
+    </row>
+    <row r="240">
+      <c r="A240" t="inlineStr">
+        <is>
+          <t>numbhh</t>
+        </is>
+      </c>
+    </row>
+    <row r="241">
+      <c r="A241" t="inlineStr">
+        <is>
+          <t>numcars</t>
+        </is>
+      </c>
+    </row>
+    <row r="242">
+      <c r="A242" t="inlineStr">
+        <is>
+          <t>outdoor</t>
+        </is>
+      </c>
+    </row>
+    <row r="243">
+      <c r="A243" t="inlineStr">
+        <is>
+          <t>pa1</t>
+        </is>
+      </c>
+    </row>
+    <row r="244">
+      <c r="A244" t="inlineStr">
+        <is>
+          <t>Perception</t>
+        </is>
+      </c>
+    </row>
+    <row r="245">
+      <c r="A245" t="inlineStr">
+        <is>
+          <t>previoustenure</t>
+        </is>
+      </c>
+    </row>
+    <row r="246">
+      <c r="A246" t="inlineStr">
+        <is>
+          <t>ra1</t>
+        </is>
+      </c>
+    </row>
+    <row r="247">
+      <c r="A247" t="inlineStr">
+        <is>
+          <t>ra15_2017</t>
+        </is>
+      </c>
+    </row>
+    <row r="248">
+      <c r="A248" t="inlineStr">
+        <is>
+          <t>ra15a</t>
+        </is>
+      </c>
+    </row>
+    <row r="249">
+      <c r="A249" t="inlineStr">
+        <is>
+          <t>ra15b</t>
+        </is>
+      </c>
+    </row>
+    <row r="250">
+      <c r="A250" t="inlineStr">
+        <is>
+          <t>ra15c</t>
+        </is>
+      </c>
+    </row>
+    <row r="251">
+      <c r="A251" t="inlineStr">
+        <is>
+          <t>rahl2</t>
+        </is>
+      </c>
+    </row>
+    <row r="252">
+      <c r="A252" t="inlineStr">
+        <is>
+          <t>rand_id</t>
+        </is>
+      </c>
+      <c r="B252" t="inlineStr">
+        <is>
+          <t>Sexual orientation</t>
+        </is>
+      </c>
+    </row>
+    <row r="253">
+      <c r="A253" t="inlineStr">
+        <is>
+          <t>randeth</t>
+        </is>
+      </c>
+      <c r="B253" t="inlineStr">
+        <is>
+          <t>Ethnicity</t>
+        </is>
+      </c>
+    </row>
+    <row r="254">
+      <c r="A254" t="inlineStr">
+        <is>
+          <t>randstat</t>
+        </is>
+      </c>
+      <c r="B254" t="inlineStr">
+        <is>
+          <t>Marital status</t>
+        </is>
+      </c>
+    </row>
+    <row r="255">
+      <c r="A255" t="inlineStr">
+        <is>
+          <t>rb1</t>
+        </is>
+      </c>
+    </row>
+    <row r="256">
+      <c r="A256" t="inlineStr">
+        <is>
+          <t>RESIL1</t>
+        </is>
+      </c>
+    </row>
+    <row r="257">
+      <c r="A257" t="inlineStr">
+        <is>
+          <t>response</t>
+        </is>
+      </c>
+    </row>
+    <row r="258">
+      <c r="A258" t="inlineStr">
+        <is>
+          <t>RESPONSE</t>
+        </is>
+      </c>
+    </row>
+    <row r="259">
+      <c r="A259" t="inlineStr">
+        <is>
+          <t>rg5a</t>
+        </is>
+      </c>
+      <c r="B259" t="inlineStr">
+        <is>
+          <t>Long-term physical or mental health condition</t>
+        </is>
+      </c>
+    </row>
+    <row r="260">
+      <c r="A260" t="inlineStr">
+        <is>
+          <t>rndrel09</t>
+        </is>
+      </c>
+      <c r="B260" t="inlineStr">
+        <is>
+          <t>Religious and ethnic belonging</t>
+        </is>
+      </c>
+    </row>
+    <row r="261">
+      <c r="A261" t="inlineStr">
+        <is>
+          <t>shs_6cla</t>
+        </is>
+      </c>
+      <c r="B261" t="inlineStr">
+        <is>
+          <t>Urban/rural classification</t>
+        </is>
+      </c>
+    </row>
+    <row r="262">
+      <c r="A262" t="inlineStr">
+        <is>
+          <t>SIMDquintiles</t>
+        </is>
+      </c>
+      <c r="B262" t="inlineStr">
+        <is>
+          <t>SIMD Quintiles</t>
+        </is>
+      </c>
+    </row>
+    <row r="263">
+      <c r="A263" t="inlineStr">
+        <is>
+          <t>social1</t>
+        </is>
+      </c>
+    </row>
+    <row r="264">
+      <c r="A264" t="inlineStr">
+        <is>
+          <t>social2</t>
+        </is>
+      </c>
+    </row>
+    <row r="265">
+      <c r="A265" t="inlineStr">
+        <is>
+          <t>tenure</t>
+        </is>
+      </c>
+      <c r="B265" t="inlineStr">
+        <is>
+          <t>Tenure</t>
+        </is>
+      </c>
+    </row>
+    <row r="266">
+      <c r="A266" t="inlineStr">
+        <is>
+          <t>tenurealt</t>
+        </is>
+      </c>
+    </row>
+    <row r="267">
+      <c r="A267" t="inlineStr">
+        <is>
+          <t>tothinc</t>
+        </is>
+      </c>
+    </row>
+    <row r="268">
+      <c r="A268" t="inlineStr">
+        <is>
+          <t>var</t>
+        </is>
+      </c>
+    </row>
+    <row r="269">
+      <c r="A269" t="inlineStr">
+        <is>
+          <t>vol32018</t>
+        </is>
+      </c>
+    </row>
+    <row r="270">
+      <c r="A270" t="inlineStr">
+        <is>
+          <t>vol42018</t>
+        </is>
+      </c>
+    </row>
+    <row r="271">
+      <c r="A271" t="inlineStr">
+        <is>
+          <t>volinform</t>
+        </is>
+      </c>
+    </row>
+    <row r="272">
+      <c r="A272" t="inlineStr">
+        <is>
+          <t>voliv2</t>
+        </is>
+      </c>
+    </row>
+    <row r="273">
+      <c r="A273" t="inlineStr">
+        <is>
+          <t>voliv3</t>
+        </is>
+      </c>
+    </row>
+    <row r="274">
+      <c r="A274" t="inlineStr">
+        <is>
+          <t>voluntee</t>
+        </is>
+      </c>
+    </row>
+    <row r="275">
+      <c r="A275" t="inlineStr">
+        <is>
+          <t>working_adults</t>
+        </is>
+      </c>
+    </row>
+    <row r="276">
+      <c r="A276" t="inlineStr">
+        <is>
+          <t>Workingageadults</t>
+        </is>
+      </c>
+      <c r="B276" t="inlineStr">
+        <is>
+          <t>Working age adults</t>
+        </is>
+      </c>
+    </row>
+    <row r="277">
+      <c r="A277" t="inlineStr">
+        <is>
+          <t>Year</t>
         </is>
       </c>
     </row>

</xml_diff>